<commit_message>
edit bugrep and chcklst
</commit_message>
<xml_diff>
--- a/BagReport_Vadim_HW.xlsx
+++ b/BagReport_Vadim_HW.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504"/>
+    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Name" sheetId="1" r:id="rId1"/>
+    <sheet name="Surname" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -152,13 +152,170 @@
   </si>
   <si>
     <t>BUG_07</t>
+  </si>
+  <si>
+    <t>BUG_08</t>
+  </si>
+  <si>
+    <t>Форма “IT Career Today web form” не проходит валидацию,при валидном заполнении всей формы, кроме поля "Surname" с одной буквой (латиницы)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Зайти на сайт  </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Форма “IT Career Today web form” не проходит валидацию.Появляется сообщение об ошибке “Заполните обязательные поля”.</t>
+  </si>
+  <si>
+    <t>BUG_09</t>
+  </si>
+  <si>
+    <t>BUG_10</t>
+  </si>
+  <si>
+    <t>BUG_11</t>
+  </si>
+  <si>
+    <t>BUG_12</t>
+  </si>
+  <si>
+    <t>BUG_13</t>
+  </si>
+  <si>
+    <t>BUG_14</t>
+  </si>
+  <si>
+    <t>BUG_15</t>
+  </si>
+  <si>
+    <t>Форма “IT Career Today web form” не проходит валидацию,при валидном заполнении всей формы, кроме поля "Surname" с двумя буквами (латиницы)</t>
+  </si>
+  <si>
+    <t>Форма “IT Career Today web form” не проходит валидацию,при валидном заполнении всей формы, кроме поля "Surname" с тремя буквами (латиницы)</t>
+  </si>
+  <si>
+    <t>Форма “IT Career Today web form” не проходит валидацию,при валидном заполнении всей формы, кроме поля "Surname" c максимальным количеством латинских букв (128)</t>
+  </si>
+  <si>
+    <t>Форма “IT Career Today web form” не проходит валидацию,при валидном заполнении всей формы, кроме поля "Surname" c максимальным количеством латинских букв (127)</t>
+  </si>
+  <si>
+    <t>Форма “IT Career Today web form” не проходит валидацию,при валидном заполнении всей формы, кроме поля "Surname" c одним разрешенным спец.символом</t>
+  </si>
+  <si>
+    <t>BUG_16</t>
+  </si>
+  <si>
+    <t>BUG_17</t>
+  </si>
+  <si>
+    <t>BUG_18</t>
+  </si>
+  <si>
+    <t>1. Заполнить поле “Name”: ”Sych”
+2. Заполнить поле “Surname”: ”q”
+3. Заполнить поле "Email": "sych@mail.ru"
+4. Заполить поле "Password": "123654"                                             
+5. Нажать кнопку "Submit"</t>
+  </si>
+  <si>
+    <t>1. Заполнить поле “Name”: ”Sych”
+2. Заполнить поле “Surname”: ”Qq”
+3. Заполнить поле "Email": "sych@mail.ru"
+4. Заполить поле "Password": "123654"                                             
+5. Нажать кнопку "Submit"</t>
+  </si>
+  <si>
+    <t>1. Заполнить поле “Name”: ”Sych”
+2. Заполнить поле “Surname”: ”Qqg”
+3. Заполнить поле "Email": "sych@mail.ru"
+4. Заполить поле "Password": "123654"                                             
+5. Нажать кнопку "Submit"</t>
+  </si>
+  <si>
+    <t>1. Заполнить поле “Name”: ”Sych”
+2. Заполнить поле “Surname”: ”Sychi@k”
+3. Заполнить поле "Email": "sych@mail.ru"
+4. Заполить поле "Password": "123654"                                             
+5. Нажать кнопку "Submit"</t>
+  </si>
+  <si>
+    <t>Форма “IT Career Today web form” проходит валидацию,при валидном заполнении всей формы, кроме поля "Surname" c буквами латиницы и запрещёнными спец.символами</t>
+  </si>
+  <si>
+    <t>1. Заполнить поле “Name”: ”Sych”
+2. Заполнить поле “Surname”: ”Sychi:k”
+3. Заполнить поле "Email": "sych@mail.ru"
+4. Заполить поле "Password": "123654"                                             
+5. Нажать кнопку "Submit"</t>
+  </si>
+  <si>
+    <t>1. Заполнить поле “Name”: ”Sych”
+2. Заполнить поле “Surname”: ”Sychi?k”
+3. Заполнить поле "Email": "sych@mail.ru"
+4. Заполить поле "Password": "123654"                                             
+5. Нажать кнопку "Submit"</t>
+  </si>
+  <si>
+    <t>1. Заполнить поле “Name”: ”Sych”
+2. Заполнить поле “Surname”: ”Sychi!k”
+3. Заполнить поле "Email": "sych@mail.ru"
+4. Заполить поле "Password": "123654"                                             
+5. Нажать кнопку "Submit"</t>
+  </si>
+  <si>
+    <t>Форма “IT Career Today web form”  проходит валидацию. Появляется сообщение об успешной регистрации.</t>
+  </si>
+  <si>
+    <t>1. Заполнить поле “Name”: ”Sych”
+2. Заполнить поле “Surname”: ”fhhhhhhhhhhhhhhdkdddddddaslkjflsifjlsifhsidlfjlsdfjosdifjosdifjiodhffhhhhhhhhhhhhhhdkdddddddaslkjflsifjlsifhsidlfjlsdfjosdifjosd”
+3. Заполнить поле "Email": "sych@mail.ru"
+4. Заполить поле "Password": "123654"                                             
+5. Нажать кнопку "Submit"</t>
+  </si>
+  <si>
+    <t>Форма “IT Career Today web form” не проходит валидацию.Незаполненные поля подсвечиваются. Появляется сообщение об ошибке “Заполните обязательные поля”.</t>
+  </si>
+  <si>
+    <t>1. Заполнить поле “Name”: ”Sych”
+2. Заполнить поле “Surname”: ”fhhhhhhhhhhhhhhdkdddddddaslkjflsifjlsifhsidlfjlsdfjosdifjosdifjiodhffhhhhhhhhhhhhhhdkdddddddaslkjflsifjlsifhsidlfjlsdfjosdifjos”
+3. Заполнить поле "Email": "sych@mail.ru"
+4. Заполить поле "Password": "123654"                                             
+5. Нажать кнопку "Submit"</t>
+  </si>
+  <si>
+    <t>1. Заполнить поле “Name”: ”Sych”
+2. Заполнить поле “Surname”: ”Sychi11k”
+3. Заполнить поле "Email": "sych@mail.ru"
+4. Заполить поле "Password": "123654"                                             
+5. Нажать кнопку "Submit"</t>
+  </si>
+  <si>
+    <t>Форма “IT Career Today web form” проходит валидацию,при валидном заполнении всей формы, кроме поля "Surname" c буквами латиницы и цифрами</t>
+  </si>
+  <si>
+    <t>1. Заполнить поле “Name”: ”Sych”
+2. Заполнить поле “Surname”: ”.”
+3. Заполнить поле "Email": "sych@mail.ru"
+4. Заполить поле "Password": "123654"                                             
+5. Нажать кнопку "Submit"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,8 +367,59 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFB45F06"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,8 +432,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -259,6 +473,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -267,7 +494,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -293,6 +520,40 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -591,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -636,7 +897,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="86.4">
+    <row r="3" spans="1:8" ht="72">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -838,13 +1099,367 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="12"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="97.8" customHeight="1">
+      <c r="A2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="92.4">
+      <c r="A3" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" ht="92.4">
+      <c r="A4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="105.6">
+      <c r="A5" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="105.6">
+      <c r="A6" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="105.6">
+      <c r="A7" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="105.6">
+      <c r="A8" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="145.19999999999999">
+      <c r="A9" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:9" ht="145.19999999999999">
+      <c r="A10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="105.6">
+      <c r="A11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="92.4">
+      <c r="A12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>